<commit_message>
Update t0.txt: add reading BPR pow and alpha values
</commit_message>
<xml_diff>
--- a/STOCH/data.xlsx
+++ b/STOCH/data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitCodes\OpenTransportData\STOCH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB6EC12-3F26-4D09-9F4C-83CEA105B1C2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C78625-1AB1-4D7C-BACB-67BEA81375B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="t0" sheetId="1" r:id="rId1"/>
     <sheet name="linkdata" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -76,9 +77,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -365,7 +367,7 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -375,13 +377,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33917A86-F1BB-4F1B-919D-048E1927CD8C}">
   <dimension ref="D2:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -395,7 +397,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D3">
         <v>1</v>
       </c>
@@ -409,7 +411,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D4">
         <v>1</v>
       </c>
@@ -423,7 +425,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="5" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>2</v>
       </c>
@@ -437,7 +439,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>2</v>
       </c>
@@ -451,7 +453,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>3</v>
       </c>
@@ -465,7 +467,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="8" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>4</v>
       </c>
@@ -479,7 +481,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>4</v>
       </c>
@@ -493,7 +495,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="10" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D10">
         <v>5</v>
       </c>
@@ -507,7 +509,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D11">
         <v>5</v>
       </c>
@@ -521,7 +523,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D12">
         <v>6</v>
       </c>
@@ -535,7 +537,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D13">
         <v>7</v>
       </c>
@@ -549,7 +551,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="14" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D14">
         <v>8</v>
       </c>
@@ -561,6 +563,153 @@
       </c>
       <c r="G14" s="1">
         <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C6A3C3B-863C-48F0-B69C-C8BAF192B7D6}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>2</v>
+      </c>
+      <c r="B9" s="2">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>2</v>
+      </c>
+      <c r="B10" s="2">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>2</v>
+      </c>
+      <c r="B11" s="2">
+        <v>4</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2">
+        <v>4</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>